<commit_message>
added AIM 429 templates
</commit_message>
<xml_diff>
--- a/Database Examples/429/_template_AIM_429.xlsx
+++ b/Database Examples/429/_template_AIM_429.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\GIT\Ballard-Arinc-429-XML-Generator\Database Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\GIT\Ballard-Arinc-429-XML-Generator\Database Examples\429\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3228D73C-A70F-488A-A46D-9DB2C2CD4E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48458584-EFC8-4619-9E79-A339A8C2DA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="6630" windowWidth="27720" windowHeight="10200" xr2:uid="{C4FFA9CA-FD51-49DE-890F-D5CB7111E100}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C4FFA9CA-FD51-49DE-890F-D5CB7111E100}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1013,7 +1013,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1024,7 +1024,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>28</v>
@@ -1187,7 +1187,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>28</v>
@@ -1250,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>29</v>
@@ -1312,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>29</v>

</xml_diff>